<commit_message>
Lab 3 report complete, optimization finished
</commit_message>
<xml_diff>
--- a/UF/COP3503/lab3/lab3data.xlsx
+++ b/UF/COP3503/lab3/lab3data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unit0\Desktop\Python\projects\UF\COP3503\lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFE015E-2389-4A3E-86D6-63FE0290440C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7604AA9B-2B9B-441D-8AAC-EDFC706C2521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="12">
   <si>
     <t>Scale Factor</t>
   </si>
@@ -392,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3310,14 +3310,2438 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72BC5550-3D14-448B-A790-26C7EE90B96C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2">
+        <v>10000000</v>
+      </c>
+      <c r="E2">
+        <v>39</v>
+      </c>
+      <c r="F2">
+        <v>9.1472700000000004E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+      <c r="D3">
+        <v>10000000</v>
+      </c>
+      <c r="E3">
+        <v>39</v>
+      </c>
+      <c r="F3">
+        <v>0.107992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1.5</v>
+      </c>
+      <c r="D4">
+        <v>10000000</v>
+      </c>
+      <c r="E4">
+        <v>39</v>
+      </c>
+      <c r="F4">
+        <v>9.3547099999999994E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>1.5</v>
+      </c>
+      <c r="D5">
+        <v>10000000</v>
+      </c>
+      <c r="E5">
+        <v>39</v>
+      </c>
+      <c r="F5">
+        <v>0.109444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>1.5</v>
+      </c>
+      <c r="D6">
+        <v>30000000</v>
+      </c>
+      <c r="E6">
+        <v>42</v>
+      </c>
+      <c r="F6">
+        <v>2.9969299999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>1.5</v>
+      </c>
+      <c r="D7">
+        <v>30000000</v>
+      </c>
+      <c r="E7">
+        <v>42</v>
+      </c>
+      <c r="F7">
+        <v>0.34005999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>1.5</v>
+      </c>
+      <c r="D8">
+        <v>30000000</v>
+      </c>
+      <c r="E8">
+        <v>42</v>
+      </c>
+      <c r="F8">
+        <v>0.282196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>1.5</v>
+      </c>
+      <c r="D9">
+        <v>30000000</v>
+      </c>
+      <c r="E9">
+        <v>42</v>
+      </c>
+      <c r="F9">
+        <v>0.33746199999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>1.5</v>
+      </c>
+      <c r="D10">
+        <v>50000000</v>
+      </c>
+      <c r="E10">
+        <v>43</v>
+      </c>
+      <c r="F10">
+        <v>0.46581699999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>1.5</v>
+      </c>
+      <c r="D11">
+        <v>50000000</v>
+      </c>
+      <c r="E11">
+        <v>43</v>
+      </c>
+      <c r="F11">
+        <v>0.55119510000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>1.5</v>
+      </c>
+      <c r="D12">
+        <v>50000000</v>
+      </c>
+      <c r="E12">
+        <v>43</v>
+      </c>
+      <c r="F12">
+        <v>0.45770100000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>1.5</v>
+      </c>
+      <c r="D13">
+        <v>50000000</v>
+      </c>
+      <c r="E13">
+        <v>43</v>
+      </c>
+      <c r="F13">
+        <v>0.55209699999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>1.5</v>
+      </c>
+      <c r="D14">
+        <v>75000000</v>
+      </c>
+      <c r="E14">
+        <v>44</v>
+      </c>
+      <c r="F14">
+        <v>0.69260500000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>1.5</v>
+      </c>
+      <c r="D15">
+        <v>75000000</v>
+      </c>
+      <c r="E15">
+        <v>44</v>
+      </c>
+      <c r="F15">
+        <v>0.79996599999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>1.5</v>
+      </c>
+      <c r="D16">
+        <v>75000000</v>
+      </c>
+      <c r="E16">
+        <v>44</v>
+      </c>
+      <c r="F16">
+        <v>0.67807899999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>1.5</v>
+      </c>
+      <c r="D17">
+        <v>75000000</v>
+      </c>
+      <c r="E17">
+        <v>44</v>
+      </c>
+      <c r="F17">
+        <v>0.770459</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>1.5</v>
+      </c>
+      <c r="D18">
+        <v>100000000</v>
+      </c>
+      <c r="E18">
+        <v>45</v>
+      </c>
+      <c r="F18">
+        <v>0.988514</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>1.5</v>
+      </c>
+      <c r="D19">
+        <v>100000000</v>
+      </c>
+      <c r="E19">
+        <v>45</v>
+      </c>
+      <c r="F19">
+        <v>1.1018300000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>1.5</v>
+      </c>
+      <c r="D20">
+        <v>100000000</v>
+      </c>
+      <c r="E20">
+        <v>45</v>
+      </c>
+      <c r="F20">
+        <v>0.96968799999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>1.5</v>
+      </c>
+      <c r="D21">
+        <v>100000000</v>
+      </c>
+      <c r="E21">
+        <v>45</v>
+      </c>
+      <c r="F21">
+        <v>1.0895900000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>10000000</v>
+      </c>
+      <c r="E22">
+        <v>23</v>
+      </c>
+      <c r="F22">
+        <v>8.3840799999999993E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>10000000</v>
+      </c>
+      <c r="E23">
+        <v>24</v>
+      </c>
+      <c r="F23">
+        <v>9.3880400000000003E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>10000000</v>
+      </c>
+      <c r="E24">
+        <v>23</v>
+      </c>
+      <c r="F24">
+        <v>7.6548400000000003E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>10000000</v>
+      </c>
+      <c r="E25">
+        <v>24</v>
+      </c>
+      <c r="F25">
+        <v>9.2738100000000004E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>30000000</v>
+      </c>
+      <c r="E26">
+        <v>24</v>
+      </c>
+      <c r="F26">
+        <v>0.19103700000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>30000000</v>
+      </c>
+      <c r="E27">
+        <v>25</v>
+      </c>
+      <c r="F27">
+        <v>0.22304199999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>30000000</v>
+      </c>
+      <c r="E28">
+        <v>24</v>
+      </c>
+      <c r="F28">
+        <v>0.185727</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>30000000</v>
+      </c>
+      <c r="E29">
+        <v>25</v>
+      </c>
+      <c r="F29">
+        <v>0.23149400000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>50000000</v>
+      </c>
+      <c r="E30">
+        <v>25</v>
+      </c>
+      <c r="F30">
+        <v>0.33935300000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>50000000</v>
+      </c>
+      <c r="E31">
+        <v>26</v>
+      </c>
+      <c r="F31">
+        <v>0.40893800000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>50000000</v>
+      </c>
+      <c r="E32">
+        <v>25</v>
+      </c>
+      <c r="F32">
+        <v>0.32920100000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>50000000</v>
+      </c>
+      <c r="E33">
+        <v>26</v>
+      </c>
+      <c r="F33">
+        <v>0.393704</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>75000000</v>
+      </c>
+      <c r="E34">
+        <v>26</v>
+      </c>
+      <c r="F34">
+        <v>0.58074599999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>75000000</v>
+      </c>
+      <c r="E35">
+        <v>27</v>
+      </c>
+      <c r="F35">
+        <v>0.66841200000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>75000000</v>
+      </c>
+      <c r="E36">
+        <v>26</v>
+      </c>
+      <c r="F36">
+        <v>0.56131500000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>75000000</v>
+      </c>
+      <c r="E37">
+        <v>27</v>
+      </c>
+      <c r="F37">
+        <v>0.67625100000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>100000000</v>
+      </c>
+      <c r="E38">
+        <v>26</v>
+      </c>
+      <c r="F38">
+        <v>0.66211399999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>100000000</v>
+      </c>
+      <c r="E39">
+        <v>27</v>
+      </c>
+      <c r="F39">
+        <v>0.77876199999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>100000000</v>
+      </c>
+      <c r="E40">
+        <v>26</v>
+      </c>
+      <c r="F40">
+        <v>0.65361999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>100000000</v>
+      </c>
+      <c r="E41">
+        <v>27</v>
+      </c>
+      <c r="F41">
+        <v>0.80124600000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>10000000</v>
+      </c>
+      <c r="E42">
+        <v>15</v>
+      </c>
+      <c r="F42">
+        <v>7.9003000000000004E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>10000000</v>
+      </c>
+      <c r="E43">
+        <v>16</v>
+      </c>
+      <c r="F43">
+        <v>8.4192400000000001E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>10000000</v>
+      </c>
+      <c r="E44">
+        <v>15</v>
+      </c>
+      <c r="F44">
+        <v>7.1605299999999997E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>10000000</v>
+      </c>
+      <c r="E45">
+        <v>16</v>
+      </c>
+      <c r="F45">
+        <v>8.3857600000000004E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>30000000</v>
+      </c>
+      <c r="E46">
+        <v>16</v>
+      </c>
+      <c r="F46">
+        <v>0.21457799999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>30000000</v>
+      </c>
+      <c r="E47">
+        <v>17</v>
+      </c>
+      <c r="F47">
+        <v>0.24817</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>30000000</v>
+      </c>
+      <c r="E48">
+        <v>16</v>
+      </c>
+      <c r="F48">
+        <v>0.21674599999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>30000000</v>
+      </c>
+      <c r="E49">
+        <v>17</v>
+      </c>
+      <c r="F49">
+        <v>0.25690600000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>50000000</v>
+      </c>
+      <c r="E50">
+        <v>16</v>
+      </c>
+      <c r="F50">
+        <v>0.28470099999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <v>50000000</v>
+      </c>
+      <c r="E51">
+        <v>17</v>
+      </c>
+      <c r="F51">
+        <v>0.34112599999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <v>50000000</v>
+      </c>
+      <c r="E52">
+        <v>16</v>
+      </c>
+      <c r="F52">
+        <v>0.27423399999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>50000000</v>
+      </c>
+      <c r="E53">
+        <v>17</v>
+      </c>
+      <c r="F53">
+        <v>0.34501799999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <v>75000000</v>
+      </c>
+      <c r="E54">
+        <v>16</v>
+      </c>
+      <c r="F54">
+        <v>0.37960500000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>75000000</v>
+      </c>
+      <c r="E55">
+        <v>17</v>
+      </c>
+      <c r="F55">
+        <v>0.46109099999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56">
+        <v>75000000</v>
+      </c>
+      <c r="E56">
+        <v>16</v>
+      </c>
+      <c r="F56">
+        <v>0.37313000000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57">
+        <v>75000000</v>
+      </c>
+      <c r="E57">
+        <v>17</v>
+      </c>
+      <c r="F57">
+        <v>0.48271900000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58">
+        <v>100000000</v>
+      </c>
+      <c r="E58">
+        <v>17</v>
+      </c>
+      <c r="F58">
+        <v>0.66125500000000004</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59">
+        <v>3</v>
+      </c>
+      <c r="D59">
+        <v>100000000</v>
+      </c>
+      <c r="E59">
+        <v>18</v>
+      </c>
+      <c r="F59">
+        <v>0.78164900000000004</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60">
+        <v>100000000</v>
+      </c>
+      <c r="E60">
+        <v>17</v>
+      </c>
+      <c r="F60">
+        <v>0.64690199999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
+        <v>100000000</v>
+      </c>
+      <c r="E61">
+        <v>18</v>
+      </c>
+      <c r="F61">
+        <v>0.80536099999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <v>10</v>
+      </c>
+      <c r="D62">
+        <v>10000000</v>
+      </c>
+      <c r="E62">
+        <v>7</v>
+      </c>
+      <c r="F62">
+        <v>4.8792299999999997E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63">
+        <v>10</v>
+      </c>
+      <c r="D63">
+        <v>10000000</v>
+      </c>
+      <c r="E63">
+        <v>8</v>
+      </c>
+      <c r="F63">
+        <v>6.04769E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64">
+        <v>10</v>
+      </c>
+      <c r="D64">
+        <v>10000000</v>
+      </c>
+      <c r="E64">
+        <v>7</v>
+      </c>
+      <c r="F64">
+        <v>4.1574300000000002E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65">
+        <v>10</v>
+      </c>
+      <c r="D65">
+        <v>10000000</v>
+      </c>
+      <c r="E65">
+        <v>8</v>
+      </c>
+      <c r="F65">
+        <v>6.2163099999999999E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66">
+        <v>10</v>
+      </c>
+      <c r="D66">
+        <v>30000000</v>
+      </c>
+      <c r="E66">
+        <v>8</v>
+      </c>
+      <c r="F66">
+        <v>0.164995</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67">
+        <v>10</v>
+      </c>
+      <c r="D67">
+        <v>30000000</v>
+      </c>
+      <c r="E67">
+        <v>9</v>
+      </c>
+      <c r="F67">
+        <v>0.20095199999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68">
+        <v>10</v>
+      </c>
+      <c r="D68">
+        <v>30000000</v>
+      </c>
+      <c r="E68">
+        <v>8</v>
+      </c>
+      <c r="F68">
+        <v>0.15437100000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69">
+        <v>10</v>
+      </c>
+      <c r="D69">
+        <v>30000000</v>
+      </c>
+      <c r="E69">
+        <v>9</v>
+      </c>
+      <c r="F69">
+        <v>0.205924</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70">
+        <v>10</v>
+      </c>
+      <c r="D70">
+        <v>50000000</v>
+      </c>
+      <c r="E70">
+        <v>8</v>
+      </c>
+      <c r="F70">
+        <v>0.23815700000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71">
+        <v>10</v>
+      </c>
+      <c r="D71">
+        <v>50000000</v>
+      </c>
+      <c r="E71">
+        <v>9</v>
+      </c>
+      <c r="F71">
+        <v>0.29333500000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <v>10</v>
+      </c>
+      <c r="D72">
+        <v>50000000</v>
+      </c>
+      <c r="E72">
+        <v>8</v>
+      </c>
+      <c r="F72">
+        <v>0.22364400000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="D73">
+        <v>50000000</v>
+      </c>
+      <c r="E73">
+        <v>9</v>
+      </c>
+      <c r="F73">
+        <v>0.30993500000000002</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74">
+        <v>10</v>
+      </c>
+      <c r="D74">
+        <v>75000000</v>
+      </c>
+      <c r="E74">
+        <v>8</v>
+      </c>
+      <c r="F74">
+        <v>0.32633600000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75">
+        <v>10</v>
+      </c>
+      <c r="D75">
+        <v>75000000</v>
+      </c>
+      <c r="E75">
+        <v>9</v>
+      </c>
+      <c r="F75">
+        <v>0.41575099999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76">
+        <v>10</v>
+      </c>
+      <c r="D76">
+        <v>75000000</v>
+      </c>
+      <c r="E76">
+        <v>8</v>
+      </c>
+      <c r="F76">
+        <v>0.31824999999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77">
+        <v>10</v>
+      </c>
+      <c r="D77">
+        <v>75000000</v>
+      </c>
+      <c r="E77">
+        <v>9</v>
+      </c>
+      <c r="F77">
+        <v>0.42105999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78">
+        <v>10</v>
+      </c>
+      <c r="D78">
+        <v>100000000</v>
+      </c>
+      <c r="E78">
+        <v>8</v>
+      </c>
+      <c r="F78">
+        <v>0.41922700000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79">
+        <v>10</v>
+      </c>
+      <c r="D79">
+        <v>100000000</v>
+      </c>
+      <c r="E79">
+        <v>9</v>
+      </c>
+      <c r="F79">
+        <v>0.53403500000000004</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80">
+        <v>10</v>
+      </c>
+      <c r="D80">
+        <v>100000000</v>
+      </c>
+      <c r="E80">
+        <v>8</v>
+      </c>
+      <c r="F80">
+        <v>0.39277699999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" t="s">
+        <v>11</v>
+      </c>
+      <c r="C81">
+        <v>10</v>
+      </c>
+      <c r="D81">
+        <v>100000000</v>
+      </c>
+      <c r="E81">
+        <v>9</v>
+      </c>
+      <c r="F81">
+        <v>0.55635999999999997</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <v>50</v>
+      </c>
+      <c r="D82">
+        <v>10000000</v>
+      </c>
+      <c r="E82">
+        <v>4</v>
+      </c>
+      <c r="F82">
+        <v>4.2715799999999998E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83">
+        <v>50</v>
+      </c>
+      <c r="D83">
+        <v>10000000</v>
+      </c>
+      <c r="E83">
+        <v>5</v>
+      </c>
+      <c r="F83">
+        <v>5.6428300000000001E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>50</v>
+      </c>
+      <c r="D84">
+        <v>10000000</v>
+      </c>
+      <c r="E84">
+        <v>4</v>
+      </c>
+      <c r="F84">
+        <v>3.6982800000000003E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85">
+        <v>50</v>
+      </c>
+      <c r="D85">
+        <v>10000000</v>
+      </c>
+      <c r="E85">
+        <v>5</v>
+      </c>
+      <c r="F85">
+        <v>5.6544200000000003E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>4</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86">
+        <v>50</v>
+      </c>
+      <c r="D86">
+        <v>30000000</v>
+      </c>
+      <c r="E86">
+        <v>5</v>
+      </c>
+      <c r="F86">
+        <v>0.14421900000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87">
+        <v>50</v>
+      </c>
+      <c r="D87">
+        <v>30000000</v>
+      </c>
+      <c r="E87">
+        <v>6</v>
+      </c>
+      <c r="F87">
+        <v>0.18289800000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88">
+        <v>50</v>
+      </c>
+      <c r="D88">
+        <v>30000000</v>
+      </c>
+      <c r="E88">
+        <v>5</v>
+      </c>
+      <c r="F88">
+        <v>0.13622799999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89">
+        <v>50</v>
+      </c>
+      <c r="D89">
+        <v>30000000</v>
+      </c>
+      <c r="E89">
+        <v>6</v>
+      </c>
+      <c r="F89">
+        <v>0.179145</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90">
+        <v>50</v>
+      </c>
+      <c r="D90">
+        <v>50000000</v>
+      </c>
+      <c r="E90">
+        <v>5</v>
+      </c>
+      <c r="F90">
+        <v>0.21648200000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>4</v>
+      </c>
+      <c r="B91" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91">
+        <v>50</v>
+      </c>
+      <c r="D91">
+        <v>50000000</v>
+      </c>
+      <c r="E91">
+        <v>6</v>
+      </c>
+      <c r="F91">
+        <v>0.28811100000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92">
+        <v>50</v>
+      </c>
+      <c r="D92">
+        <v>50000000</v>
+      </c>
+      <c r="E92">
+        <v>5</v>
+      </c>
+      <c r="F92">
+        <v>0.206515</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" t="s">
+        <v>11</v>
+      </c>
+      <c r="C93">
+        <v>50</v>
+      </c>
+      <c r="D93">
+        <v>50000000</v>
+      </c>
+      <c r="E93">
+        <v>6</v>
+      </c>
+      <c r="F93">
+        <v>0.28278599999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>4</v>
+      </c>
+      <c r="B94" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94">
+        <v>50</v>
+      </c>
+      <c r="D94">
+        <v>75000000</v>
+      </c>
+      <c r="E94">
+        <v>5</v>
+      </c>
+      <c r="F94">
+        <v>0.30446200000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C95">
+        <v>50</v>
+      </c>
+      <c r="D95">
+        <v>75000000</v>
+      </c>
+      <c r="E95">
+        <v>6</v>
+      </c>
+      <c r="F95">
+        <v>0.39426600000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96">
+        <v>50</v>
+      </c>
+      <c r="D96">
+        <v>75000000</v>
+      </c>
+      <c r="E96">
+        <v>5</v>
+      </c>
+      <c r="F96">
+        <v>0.29785800000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97">
+        <v>50</v>
+      </c>
+      <c r="D97">
+        <v>75000000</v>
+      </c>
+      <c r="E97">
+        <v>6</v>
+      </c>
+      <c r="F97">
+        <v>0.40248800000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>4</v>
+      </c>
+      <c r="B98" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98">
+        <v>50</v>
+      </c>
+      <c r="D98">
+        <v>100000000</v>
+      </c>
+      <c r="E98">
+        <v>5</v>
+      </c>
+      <c r="F98">
+        <v>0.39472200000000002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>4</v>
+      </c>
+      <c r="B99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99">
+        <v>50</v>
+      </c>
+      <c r="D99">
+        <v>100000000</v>
+      </c>
+      <c r="E99">
+        <v>6</v>
+      </c>
+      <c r="F99">
+        <v>0.50767700000000004</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100">
+        <v>50</v>
+      </c>
+      <c r="D100">
+        <v>100000000</v>
+      </c>
+      <c r="E100">
+        <v>5</v>
+      </c>
+      <c r="F100">
+        <v>0.36856899999999998</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" t="s">
+        <v>11</v>
+      </c>
+      <c r="C101">
+        <v>50</v>
+      </c>
+      <c r="D101">
+        <v>100000000</v>
+      </c>
+      <c r="E101">
+        <v>6</v>
+      </c>
+      <c r="F101">
+        <v>0.52167399999999997</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102">
+        <v>100</v>
+      </c>
+      <c r="D102">
+        <v>10000000</v>
+      </c>
+      <c r="E102">
+        <v>4</v>
+      </c>
+      <c r="F102">
+        <v>4.87562E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103">
+        <v>100</v>
+      </c>
+      <c r="D103">
+        <v>10000000</v>
+      </c>
+      <c r="E103">
+        <v>5</v>
+      </c>
+      <c r="F103">
+        <v>5.9408099999999998E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104">
+        <v>100</v>
+      </c>
+      <c r="D104">
+        <v>10000000</v>
+      </c>
+      <c r="E104">
+        <v>4</v>
+      </c>
+      <c r="F104">
+        <v>4.3026399999999999E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105" t="s">
+        <v>11</v>
+      </c>
+      <c r="C105">
+        <v>100</v>
+      </c>
+      <c r="D105">
+        <v>10000000</v>
+      </c>
+      <c r="E105">
+        <v>5</v>
+      </c>
+      <c r="F105">
+        <v>5.9717899999999997E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106">
+        <v>100</v>
+      </c>
+      <c r="D106">
+        <v>30000000</v>
+      </c>
+      <c r="E106">
+        <v>4</v>
+      </c>
+      <c r="F106">
+        <v>0.13569300000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>4</v>
+      </c>
+      <c r="B107" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107">
+        <v>100</v>
+      </c>
+      <c r="D107">
+        <v>30000000</v>
+      </c>
+      <c r="E107">
+        <v>5</v>
+      </c>
+      <c r="F107">
+        <v>0.153198</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108">
+        <v>100</v>
+      </c>
+      <c r="D108">
+        <v>30000000</v>
+      </c>
+      <c r="E108">
+        <v>4</v>
+      </c>
+      <c r="F108">
+        <v>0.11034099999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109">
+        <v>100</v>
+      </c>
+      <c r="D109">
+        <v>30000000</v>
+      </c>
+      <c r="E109">
+        <v>5</v>
+      </c>
+      <c r="F109">
+        <v>0.16073200000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>4</v>
+      </c>
+      <c r="B110" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110">
+        <v>100</v>
+      </c>
+      <c r="D110">
+        <v>50000000</v>
+      </c>
+      <c r="E110">
+        <v>4</v>
+      </c>
+      <c r="F110">
+        <v>0.19484799999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>4</v>
+      </c>
+      <c r="B111" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111">
+        <v>100</v>
+      </c>
+      <c r="D111">
+        <v>50000000</v>
+      </c>
+      <c r="E111">
+        <v>5</v>
+      </c>
+      <c r="F111">
+        <v>0.25234800000000002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" t="s">
+        <v>10</v>
+      </c>
+      <c r="C112">
+        <v>100</v>
+      </c>
+      <c r="D112">
+        <v>50000000</v>
+      </c>
+      <c r="E112">
+        <v>4</v>
+      </c>
+      <c r="F112">
+        <v>0.17897099999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113" t="s">
+        <v>11</v>
+      </c>
+      <c r="C113">
+        <v>100</v>
+      </c>
+      <c r="D113">
+        <v>50000000</v>
+      </c>
+      <c r="E113">
+        <v>5</v>
+      </c>
+      <c r="F113">
+        <v>0.26057200000000003</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>4</v>
+      </c>
+      <c r="B114" t="s">
+        <v>8</v>
+      </c>
+      <c r="C114">
+        <v>100</v>
+      </c>
+      <c r="D114">
+        <v>75000000</v>
+      </c>
+      <c r="E114">
+        <v>4</v>
+      </c>
+      <c r="F114">
+        <v>0.28040900000000002</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>4</v>
+      </c>
+      <c r="B115" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115">
+        <v>100</v>
+      </c>
+      <c r="D115">
+        <v>75000000</v>
+      </c>
+      <c r="E115">
+        <v>5</v>
+      </c>
+      <c r="F115">
+        <v>0.37042700000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>5</v>
+      </c>
+      <c r="B116" t="s">
+        <v>10</v>
+      </c>
+      <c r="C116">
+        <v>100</v>
+      </c>
+      <c r="D116">
+        <v>75000000</v>
+      </c>
+      <c r="E116">
+        <v>4</v>
+      </c>
+      <c r="F116">
+        <v>0.26594899999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117" t="s">
+        <v>11</v>
+      </c>
+      <c r="C117">
+        <v>100</v>
+      </c>
+      <c r="D117">
+        <v>75000000</v>
+      </c>
+      <c r="E117">
+        <v>5</v>
+      </c>
+      <c r="F117">
+        <v>0.37885099999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>4</v>
+      </c>
+      <c r="B118" t="s">
+        <v>8</v>
+      </c>
+      <c r="C118">
+        <v>100</v>
+      </c>
+      <c r="D118">
+        <v>100000000</v>
+      </c>
+      <c r="E118">
+        <v>4</v>
+      </c>
+      <c r="F118">
+        <v>0.37131599999999998</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>4</v>
+      </c>
+      <c r="B119" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119">
+        <v>100</v>
+      </c>
+      <c r="D119">
+        <v>100000000</v>
+      </c>
+      <c r="E119">
+        <v>5</v>
+      </c>
+      <c r="F119">
+        <v>0.49221199999999998</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120" t="s">
+        <v>10</v>
+      </c>
+      <c r="C120">
+        <v>100</v>
+      </c>
+      <c r="D120">
+        <v>100000000</v>
+      </c>
+      <c r="E120">
+        <v>4</v>
+      </c>
+      <c r="F120">
+        <v>0.36412499999999998</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>5</v>
+      </c>
+      <c r="B121" t="s">
+        <v>11</v>
+      </c>
+      <c r="C121">
+        <v>100</v>
+      </c>
+      <c r="D121">
+        <v>100000000</v>
+      </c>
+      <c r="E121">
+        <v>5</v>
+      </c>
+      <c r="F121">
+        <v>0.4995</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>